<commit_message>
BACKEND- Servicio -Proveedores-Param Clase-Categorias
</commit_message>
<xml_diff>
--- a/backEnd/documentacion/doc_servicios.xlsx
+++ b/backEnd/documentacion/doc_servicios.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\proyectos\Ventas\sales\backEnd\documentacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\proyectos\Ventas\salesforce\backEnd\documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
   <si>
     <t>Nro</t>
   </si>
@@ -211,6 +211,110 @@
   <si>
     <t>http://localhost:8089/b-salesforce/rest/unidad_medida</t>
   </si>
+  <si>
+    <t>Listado de Categorias</t>
+  </si>
+  <si>
+    <t>http://localhost:8089/b-salesforce/rest/categoria</t>
+  </si>
+  <si>
+    <t>{
+    "success": true,
+    "message": "Consulta exitosa.",
+    "result": [
+        {
+            "id": 1,
+            "descripcionCategoria": "JOYAS"
+        },
+        {
+            "id": 2,
+            "descripcionCategoria": "BOJOUTERIA"
+        },
+        {
+            "id": 3,
+            "descripcionCategoria": "INSUMOS"
+        }
+    ]
+}</t>
+  </si>
+  <si>
+    <t>GET</t>
+  </si>
+  <si>
+    <t>Listado de Clase</t>
+  </si>
+  <si>
+    <t>http://localhost:8089/b-salesforce/rest/categoria/{idCategoria}/clase</t>
+  </si>
+  <si>
+    <t>{
+    "success": true,
+    "message": "Consulta Exitosa.",
+    "result": [
+        {
+            "id": 8,
+            "descripcionClase": "GRANALLA"
+        },
+        {
+            "id": 9,
+            "descripcionClase": "POST"
+        }
+    ]
+}</t>
+  </si>
+  <si>
+    <t>Listado de proveedores</t>
+  </si>
+  <si>
+    <t>http://localhost:8089/b-salesforce/rest/proveedores</t>
+  </si>
+  <si>
+    <t>{
+    "success": true,
+    "message": "Consulta exitosa.",
+    "result": [
+        {
+            "id": 1,
+            "disabled": false,
+            "nombre": "COMPANEX SRL",
+            "numeroDocumento": "4851800011",
+            "direccion": null,
+            "telefono": "78787878",
+            "fax": "4545454545",
+            "email": "jheyson@gmail.com",
+            "contacto": "jheyson sanchez",
+            "cuenta_pp": null,
+            "cuenta_p": "1000545454"
+        },
+        {
+            "id": 2,
+            "disabled": false,
+            "nombre": "YANAPAX SRL",
+            "numeroDocumento": "48484850001",
+            "direccion": "Ave. los leones nro. 5898 Alto Obreajes",
+            "telefono": "244441225",
+            "fax": "2454545",
+            "email": "carlos@gmail.com",
+            "contacto": "carlos sanchez",
+            "cuenta_pp": null,
+            "cuenta_p": "10003232325"
+        },
+        {
+            "id": 3,
+            "disabled": false,
+            "nombre": "infoglobal",
+            "numeroDocumento": "78787878778",
+            "direccion": "calle pichincha",
+            "telefono": "2484848",
+            "fax": "2484848",
+            "email": "infoglobal@gmail.com",
+            "contacto": "carlos veltran",
+            "cuenta_pp": "787877",
+            "cuenta_p": "78787878787"
+        }
+    ]
+}</t>
+  </si>
 </sst>
 </file>
 
@@ -233,12 +337,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -254,7 +364,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -266,10 +376,16 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -552,38 +668,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AU6"/>
+  <dimension ref="A1:AU9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="25" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="57.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="67.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="45.5703125" customWidth="1"/>
     <col min="6" max="6" width="43" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
     </row>
     <row r="2" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C2" t="s">
@@ -656,7 +772,9 @@
       <c r="C5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="1"/>
+      <c r="D5" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="E5" s="1"/>
       <c r="F5" s="2" t="s">
         <v>18</v>
@@ -713,10 +831,66 @@
       <c r="C6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="1"/>
+      <c r="D6" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="E6" s="1"/>
       <c r="F6" s="2" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:47" ht="270" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>4</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:47" ht="210" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>5</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="F8" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:47" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="6">
+        <v>6</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="6"/>
+      <c r="F9" s="7" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -726,6 +900,8 @@
   <hyperlinks>
     <hyperlink ref="C3" r:id="rId1"/>
     <hyperlink ref="C6" r:id="rId2"/>
+    <hyperlink ref="C7" r:id="rId3"/>
+    <hyperlink ref="C8" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
SERVICIO TIPO MOVIMIENTO url: http://localhost:8089/b-salesforce/rest/tipoMovimiento respuesta: {     "success": true,     "message": "Consulta exitosa.",     "result": [         {             "id": 1,             "clasifMovimientos": "COMPRA",             "descripcionMovimientos": "COMPRA DE MERCANCIA"         },         {             "id": 2,             "clasifMovimientos": "VENTA",             "descripcionMovimientos": "VENTA DE MERCANCIA"         }     ] }
</commit_message>
<xml_diff>
--- a/backEnd/documentacion/doc_servicios.xlsx
+++ b/backEnd/documentacion/doc_servicios.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
   <si>
     <t>Nro</t>
   </si>
@@ -315,6 +315,30 @@
     ]
 }</t>
   </si>
+  <si>
+    <t>Listado tipo Movimiento</t>
+  </si>
+  <si>
+    <t>http://localhost:8089/b-salesforce/rest/tipoMovimiento</t>
+  </si>
+  <si>
+    <t>{
+    "success": true,
+    "message": "Consulta exitosa.",
+    "result": [
+        {
+            "id": 1,
+            "clasifMovimientos": "COMPRA",
+            "descripcionMovimientos": "COMPRA DE MERCANCIA"
+        },
+        {
+            "id": 2,
+            "clasifMovimientos": "VENTA",
+            "descripcionMovimientos": "VENTA DE MERCANCIA"
+        }
+    ]
+}</t>
+  </si>
 </sst>
 </file>
 
@@ -337,18 +361,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -378,14 +396,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -668,10 +686,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AU9"/>
+  <dimension ref="A1:AU10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:F9"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -683,17 +701,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
     </row>
     <row r="2" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -876,21 +894,39 @@
       </c>
     </row>
     <row r="9" spans="1:47" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="6">
+      <c r="A9" s="5">
         <v>6</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="6"/>
-      <c r="F9" s="7" t="s">
+      <c r="E9" s="5"/>
+      <c r="F9" s="6" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:47" ht="270" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
+        <v>7</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SERVICIO PARA EL REGISTRO DE MOVIMIENTOS COMPRA - VENTA
</commit_message>
<xml_diff>
--- a/backEnd/documentacion/doc_servicios.xlsx
+++ b/backEnd/documentacion/doc_servicios.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="41">
   <si>
     <t>Nro</t>
   </si>
@@ -335,6 +335,102 @@
             "id": 2,
             "clasifMovimientos": "VENTA",
             "descripcionMovimientos": "VENTA DE MERCANCIA"
+        }
+    ]
+}</t>
+  </si>
+  <si>
+    <t>listado de articulos habilitados</t>
+  </si>
+  <si>
+    <t>http://localhost:8089/b-salesforce/rest/articulosHabilitados</t>
+  </si>
+  <si>
+    <t>{
+    "success": true,
+    "message": "Consulta Exitosa.",
+    "result": [
+        {
+            "id": 1,
+            "descripcionArticulo": "ANILLO CUADRADO",
+            "codigoArticulo": "JOAN0.0.1",
+            "metodoCosto": "95.0",
+            "precio": 100,
+            "precioCosto": null,
+            "upc": null,
+            "nivelReorden": 0,
+            "cantidadReorden": 3,
+            "nSerie": 0,
+            "fotografia": null,
+            "fechaDesde": 1410386400000,
+            "fechaHasta": null,
+            "usuarioAct": "JSON"
+        },
+        {
+            "id": 2,
+            "descripcionArticulo": "ANILLO RECTANGULAR",
+            "codigoArticulo": "JOAN0.0.2",
+            "metodoCosto": "250.0",
+            "precio": 15000,
+            "precioCosto": null,
+            "upc": null,
+            "nivelReorden": 0,
+            "cantidadReorden": 3,
+            "nSerie": 0,
+            "fotografia": null,
+            "fechaDesde": 1410386400000,
+            "fechaHasta": null,
+            "usuarioAct": "JSON"
+        },
+        {
+            "id": 3,
+            "descripcionArticulo": "ANILLO ZEBRA",
+            "codigoArticulo": "JOAN0.0.3",
+            "metodoCosto": "500.0",
+            "precio": 2500,
+            "precioCosto": null,
+            "upc": null,
+            "nivelReorden": 0,
+            "cantidadReorden": 3,
+            "nSerie": 0,
+            "fotografia": null,
+            "fechaDesde": 1410386400000,
+            "fechaHasta": null,
+            "usuarioAct": "JSON"
+        }
+    ]
+}</t>
+  </si>
+  <si>
+    <t>Listado de proveedores habilitados</t>
+  </si>
+  <si>
+    <t>http://localhost:8089/b-salesforce/rest/proveedorMovimiento</t>
+  </si>
+  <si>
+    <t>{
+    "success": true,
+    "message": "Consulta exitosa.",
+    "result": [
+        {
+            "id": 1,
+            "nombre": "COMPANEX SRL",
+            "numeroDocumento": "4851800011"
+        },
+        {
+            "id": 2,
+            "nombre": "YANAPAX SRL",
+            "numeroDocumento": "48484850001"
+        },
+        {
+            "id": 3,
+            "nombre": "infoglobal",
+            "numeroDocumento": "78787878778"
+        },
+        {
+            "id": 4,
+            "nombre": "ENATEX",
+            "numeroDocumento": "4851800"
         }
     ]
 }</t>
@@ -686,10 +782,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AU10"/>
+  <dimension ref="A1:AU12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -929,6 +1025,42 @@
         <v>34</v>
       </c>
     </row>
+    <row r="11" spans="1:47" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
+        <v>8</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="1"/>
+      <c r="F11" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:47" ht="390" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
+        <v>9</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="1"/>
+      <c r="F12" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:I1"/>
@@ -938,6 +1070,7 @@
     <hyperlink ref="C6" r:id="rId2"/>
     <hyperlink ref="C7" r:id="rId3"/>
     <hyperlink ref="C8" r:id="rId4"/>
+    <hyperlink ref="C12" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Servicio guardar Clase con Objeto Categoria
</commit_message>
<xml_diff>
--- a/backEnd/documentacion/doc_servicios.xlsx
+++ b/backEnd/documentacion/doc_servicios.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\proyectos\Ventas\salesforce\backEnd\documentacion\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4755"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="52">
   <si>
     <t>Nro</t>
   </si>
@@ -490,6 +485,46 @@
   </si>
   <si>
     <t>Le pasas por parametro el id del articulo</t>
+  </si>
+  <si>
+    <t>guardar categoria</t>
+  </si>
+  <si>
+    <t>{
+  "descripcionClase":"CLASE PRUEBA",
+  "fechaDesde":null,
+  "fechaHasta":null,
+  "usuarioAct":"BOMBA",
+  "clasif_categoria":{
+    "id":2,
+    "descripcionCategoria":"JOYAS"
+  }
+}</t>
+  </si>
+  <si>
+    <t>{
+    "success": true,
+    "message": "Se registro satisfactoriamente.",
+    "result": {
+        "id": 10,
+        "disabled": false,
+        "descripcionClase": "CLASE PRUEBA",
+        "fechaDesde": null,
+        "fechaHasta": null,
+        "usuarioAct": "BOMBA",
+        "clasif_categoria": {
+            "id": 2,
+            "disabled": false,
+            "descripcionCategoria": "BOJOUTERIA",
+            "fechaDesde": 1411505081754,
+            "fechaHasta": 1411505081754,
+            "usuarioAct": "JSON"
+        }
+    }
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://localhost:8080/b-salesforce/rest/clases/guardar </t>
   </si>
 </sst>
 </file>
@@ -562,11 +597,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -628,7 +663,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -663,7 +698,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -840,7 +875,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -848,10 +883,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AU14"/>
+  <dimension ref="A1:AU16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -864,17 +899,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
     </row>
     <row r="2" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -1158,14 +1193,39 @@
       <c r="B14" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="8" t="s">
         <v>46</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G14" s="8" t="s">
+      <c r="G14" s="7" t="s">
         <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:47" s="1" customFormat="1" ht="315" x14ac:dyDescent="0.25">
+      <c r="A15" s="5">
+        <v>12</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A16" s="5">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1179,8 +1239,9 @@
     <hyperlink ref="C8" r:id="rId4"/>
     <hyperlink ref="C12" r:id="rId5"/>
     <hyperlink ref="C14" r:id="rId6"/>
+    <hyperlink ref="C15" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId7"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>